<commit_message>
updated figures and candidate_pairs Stats for ComEM
</commit_message>
<xml_diff>
--- a/experiments/figures/Com_EM_metrics.xlsx
+++ b/experiments/figures/Com_EM_metrics.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,7 @@
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -488,6 +489,11 @@
           <t>f1</t>
         </is>
       </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>runtime</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -504,6 +510,11 @@
       <c r="D4" t="n">
         <v>38.94273127753304</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>49:06</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -520,6 +531,11 @@
       <c r="D5" t="n">
         <v>34.39930855661193</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>29:45</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -536,6 +552,11 @@
       <c r="D6" t="n">
         <v>12.4101581217058</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>38:31</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -552,6 +573,11 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>68:43</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -568,6 +594,11 @@
       <c r="D8" t="n">
         <v>10.3036506311839</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>235:38</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -584,6 +615,11 @@
       <c r="D9" t="n">
         <v>22.0532319391635</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>141:40</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -600,6 +636,11 @@
       <c r="D10" t="n">
         <v>1.764953918438648</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>153:06</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -616,6 +657,11 @@
       <c r="D11" t="n">
         <v>8.058608058608058</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>381:42</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -632,6 +678,11 @@
       <c r="D12" t="n">
         <v>0.2864303616183316</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>213:38</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -648,6 +699,11 @@
       <c r="D13" t="n">
         <v>0.9033423667570007</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>123:00</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -664,6 +720,11 @@
       <c r="D14" t="n">
         <v>0.05412475756619</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>141:50</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -680,6 +741,11 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>389:56</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -696,6 +762,11 @@
       <c r="D16" t="n">
         <v>0.0475963826749167</v>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>214:06</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -712,6 +783,11 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>132:17</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -728,6 +804,11 @@
       <c r="D18" t="n">
         <v>0.0264557263419667</v>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>148:47</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -744,6 +825,11 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>362:45</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -760,6 +846,11 @@
       <c r="D20" t="n">
         <v>5.952243626715884</v>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>119:40</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -776,6 +867,11 @@
       <c r="D21" t="n">
         <v>22.53521126760564</v>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>72:03</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -792,6 +888,11 @@
       <c r="D22" t="n">
         <v>1.656007309273641</v>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>77:18</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -808,10 +909,15 @@
       <c r="D23" t="n">
         <v>0</v>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>195:47</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>